<commit_message>
tp 7 completo y tp8 casi terminado
</commit_message>
<xml_diff>
--- a/TP 7/punto 6.xlsx
+++ b/TP 7/punto 6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UADER\Tercero\Ingenieria de software ll\ing-sw-II\TP 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonzalo\Desktop\escritorio\tercero\ingenieria de software II\ing-sw-II\TP 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D129DB6F-7C6A-4D09-9B79-891E32734FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D25C41E-FFD9-4541-BAA6-37495D581018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10236" yWindow="2544" windowWidth="5328" windowHeight="8904" xr2:uid="{EE3B17FE-B475-47ED-A072-756EC160D192}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8832" xr2:uid="{EE3B17FE-B475-47ED-A072-756EC160D192}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -72,7 +71,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -132,14 +131,14 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -459,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3B32FC-B628-4028-B0CB-5FC68FB722EF}">
   <dimension ref="A2:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,8 +528,8 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <f>B3*B6 - B3*B7</f>
-        <v>157.20000000000005</v>
+        <f>B3-B8</f>
+        <v>828.65200000000004</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -539,7 +538,7 @@
       </c>
       <c r="B10" s="3">
         <f>B5+B9</f>
-        <v>1247.2</v>
+        <v>1918.652</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -548,7 +547,7 @@
       </c>
       <c r="B11" s="1">
         <f>((B10/B3)-1)</f>
-        <v>0.24720000000000009</v>
+        <v>0.91865200000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>